<commit_message>
CutsceneIntro: update dialogue. ChatEngine: update dialogue for LV1, 8, 34, 51, and add 125.
</commit_message>
<xml_diff>
--- a/JSON/InGameChatDialogues.xlsx
+++ b/JSON/InGameChatDialogues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA6F67E-5D50-E647-AAE2-9B7671171A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F41665F-C4C8-BF46-8160-AAE3D5E21231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{BEC1C2E6-1980-8E46-829C-045BE56B3A8A}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$1</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="81">
   <si>
     <t>Profile</t>
   </si>
@@ -209,9 +209,6 @@
     <t>Why is it always the pretty things in life that are the most deadly...</t>
   </si>
   <si>
-    <t>Don't step on the bombs. Yeah got it.</t>
-  </si>
-  <si>
     <t>OK. Now if the flashing lights become too much, you can tap the disco ball below to turn them off. 🪩 GET READY!!!</t>
   </si>
   <si>
@@ -221,29 +218,77 @@
     <t>Villain</t>
   </si>
   <si>
-    <t>You'll never find her… You can keep trying, but she serves another purpose now…</t>
-  </si>
-  <si>
-    <t>100DR2</t>
-  </si>
-  <si>
-    <t>You had your chance. Now face the consequences…</t>
-  </si>
-  <si>
-    <t>This isn't over!</t>
-  </si>
-  <si>
-    <t>We shall see...</t>
-  </si>
-  <si>
     <t>So you ARE behind this. I should have known!</t>
+  </si>
+  <si>
+    <t>That was many years ago. LET HER GO AND THINGS WON'T HAVE TO GET UGLY!!</t>
+  </si>
+  <si>
+    <t>I did what I had to do. And I'll do it again to stop you from destroying this realm.</t>
+  </si>
+  <si>
+    <t>We would have made a great duo—the strongest wizards in all the realms, but you thought only of yourself.</t>
+  </si>
+  <si>
+    <t>100DR2?</t>
+  </si>
+  <si>
+    <t>Don't step on the bombs. Yeah got it, old man.</t>
+  </si>
+  <si>
+    <t>Is everything OK?? You've been awfully quiet. You're usually chewing my ear off right about now.</t>
+  </si>
+  <si>
+    <t>Ok, ok. I'll be ready. I already know how to use swords and hammers. Nothing can stop me!</t>
+  </si>
+  <si>
+    <t>Well yeah, after I saw a friggin' dragon swoop down from a blood soaked sky and snatch a 7 year old girl, you appeared almost out of nowhere.</t>
+  </si>
+  <si>
+    <t>Look, if it's the old man comment, everybody gets old. It's just an inevitability of life. I'm 16 so everyone looks old to me.</t>
+  </si>
+  <si>
+    <t>Why are you so surprised? We're bounded by fate, as the [Dodecahedron] revealed us.</t>
+  </si>
+  <si>
+    <t>You reached out to me for my help. I need you to trust me now.</t>
+  </si>
+  <si>
+    <t>Good. Then we're in agreement. Now no more silly questions. Let's keep pushing forward.</t>
+  </si>
+  <si>
+    <t>You'll never find her... You can keep trying, but she serves another purpose now...</t>
+  </si>
+  <si>
+    <t>Such a shame. So lost. One day you'll know the truth...</t>
+  </si>
+  <si>
+    <t>...</t>
+  </si>
+  <si>
+    <t>ONE THOUSAND??!! What are you, like a wizard or something? Wait... ARE YOU?!?! Because I'm not surprised by anything anymore at this point...</t>
+  </si>
+  <si>
+    <t>No, it's not that. I'm 1,000 years old. I AM old. I'm just thinking about how important it is we complete the mission.</t>
+  </si>
+  <si>
+    <t>I mean you don't look a day over 800 to be honest...</t>
+  </si>
+  <si>
+    <t>PUZL Boy, I need you to be serious! What lies ahead will test your patience. It will make you want to throw your phone out the window. You need to be prepared!</t>
+  </si>
+  <si>
+    <t>There's a lot you must learn to prepare you for the upcoming battle to save your world and the worlds beyond your world.</t>
+  </si>
+  <si>
+    <t>Wow.. 1,000 years old. I have soooo many questions...</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -259,8 +304,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -279,6 +330,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -292,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -305,6 +368,19 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -623,10 +699,10 @@
   <dimension ref="A1:D206"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D54" sqref="D54"/>
+      <selection pane="bottomRight" activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -659,7 +735,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1">
-        <f>LEN(D2)</f>
+        <f t="shared" ref="C2:C65" si="0">LEN(D2)</f>
         <v>53</v>
       </c>
       <c r="D2" t="s">
@@ -674,7 +750,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1">
-        <f>LEN(D3)</f>
+        <f t="shared" si="0"/>
         <v>138</v>
       </c>
       <c r="D3" t="s">
@@ -689,7 +765,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <f>LEN(D4)</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="D4" t="s">
@@ -704,7 +780,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="1">
-        <f>LEN(D5)</f>
+        <f t="shared" si="0"/>
         <v>137</v>
       </c>
       <c r="D5" t="s">
@@ -719,7 +795,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1">
-        <f>LEN(D6)</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="D6" t="s">
@@ -734,7 +810,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="1">
-        <f>LEN(D7)</f>
+        <f t="shared" si="0"/>
         <v>86</v>
       </c>
       <c r="D7" t="s">
@@ -749,7 +825,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="1">
-        <f>LEN(D8)</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="D8" t="s">
@@ -764,7 +840,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="1">
-        <f>LEN(D9)</f>
+        <f t="shared" si="0"/>
         <v>131</v>
       </c>
       <c r="D9" t="s">
@@ -779,7 +855,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="1">
-        <f>LEN(D10)</f>
+        <f t="shared" si="0"/>
         <v>142</v>
       </c>
       <c r="D10" t="s">
@@ -794,7 +870,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="1">
-        <f>LEN(D11)</f>
+        <f t="shared" si="0"/>
         <v>124</v>
       </c>
       <c r="D11" t="s">
@@ -809,7 +885,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="1">
-        <f>LEN(D12)</f>
+        <f t="shared" si="0"/>
         <v>88</v>
       </c>
       <c r="D12" t="s">
@@ -824,7 +900,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="1">
-        <f>LEN(D13)</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="D13" t="s">
@@ -839,7 +915,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="1">
-        <f>LEN(D14)</f>
+        <f t="shared" si="0"/>
         <v>95</v>
       </c>
       <c r="D14" t="s">
@@ -854,7 +930,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="1">
-        <f>LEN(D15)</f>
+        <f t="shared" si="0"/>
         <v>107</v>
       </c>
       <c r="D15" t="s">
@@ -869,7 +945,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="1">
-        <f>LEN(D16)</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="D16" t="s">
@@ -884,7 +960,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="1">
-        <f>LEN(D17)</f>
+        <f t="shared" si="0"/>
         <v>77</v>
       </c>
       <c r="D17" t="s">
@@ -899,7 +975,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="1">
-        <f>LEN(D18)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="D18" t="s">
@@ -914,7 +990,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="1">
-        <f>LEN(D19)</f>
+        <f t="shared" si="0"/>
         <v>106</v>
       </c>
       <c r="D19" t="s">
@@ -929,7 +1005,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="1">
-        <f>LEN(D20)</f>
+        <f t="shared" si="0"/>
         <v>114</v>
       </c>
       <c r="D20" t="s">
@@ -944,7 +1020,7 @@
         <v>5</v>
       </c>
       <c r="C21" s="1">
-        <f>LEN(D21)</f>
+        <f t="shared" si="0"/>
         <v>59</v>
       </c>
       <c r="D21" t="s">
@@ -959,7 +1035,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="1">
-        <f>LEN(D22)</f>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="D22" t="s">
@@ -974,7 +1050,7 @@
         <v>5</v>
       </c>
       <c r="C23" s="1">
-        <f>LEN(D23)</f>
+        <f t="shared" si="0"/>
         <v>107</v>
       </c>
       <c r="D23" t="s">
@@ -989,7 +1065,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="1">
-        <f>LEN(D24)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="D24" t="s">
@@ -1004,7 +1080,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="1">
-        <f>LEN(D25)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="D25" t="s">
@@ -1019,7 +1095,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="1">
-        <f>LEN(D26)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="D26" t="s">
@@ -1034,7 +1110,7 @@
         <v>3</v>
       </c>
       <c r="C27" s="1">
-        <f>LEN(D27)</f>
+        <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="D27" t="s">
@@ -1049,7 +1125,7 @@
         <v>5</v>
       </c>
       <c r="C28" s="1">
-        <f>LEN(D28)</f>
+        <f t="shared" si="0"/>
         <v>126</v>
       </c>
       <c r="D28" t="s">
@@ -1064,7 +1140,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="1">
-        <f>LEN(D29)</f>
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="D29" t="s">
@@ -1079,7 +1155,7 @@
         <v>5</v>
       </c>
       <c r="C30" s="1">
-        <f>LEN(D30)</f>
+        <f t="shared" si="0"/>
         <v>78</v>
       </c>
       <c r="D30" t="s">
@@ -1094,7 +1170,7 @@
         <v>5</v>
       </c>
       <c r="C31" s="1">
-        <f>LEN(D31)</f>
+        <f t="shared" si="0"/>
         <v>116</v>
       </c>
       <c r="D31" t="s">
@@ -1109,7 +1185,7 @@
         <v>5</v>
       </c>
       <c r="C32" s="1">
-        <f>LEN(D32)</f>
+        <f t="shared" si="0"/>
         <v>112</v>
       </c>
       <c r="D32" t="s">
@@ -1124,7 +1200,7 @@
         <v>3</v>
       </c>
       <c r="C33" s="1">
-        <f>LEN(D33)</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="D33" t="s">
@@ -1139,7 +1215,7 @@
         <v>5</v>
       </c>
       <c r="C34" s="1">
-        <f>LEN(D34)</f>
+        <f t="shared" si="0"/>
         <v>85</v>
       </c>
       <c r="D34" t="s">
@@ -1154,7 +1230,7 @@
         <v>5</v>
       </c>
       <c r="C35" s="1">
-        <f>LEN(D35)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
       <c r="D35" t="s">
@@ -1169,7 +1245,7 @@
         <v>5</v>
       </c>
       <c r="C36" s="1">
-        <f>LEN(D36)</f>
+        <f t="shared" si="0"/>
         <v>96</v>
       </c>
       <c r="D36" t="s">
@@ -1184,7 +1260,7 @@
         <v>3</v>
       </c>
       <c r="C37" s="1">
-        <f>LEN(D37)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="D37" t="s">
@@ -1199,7 +1275,7 @@
         <v>5</v>
       </c>
       <c r="C38" s="1">
-        <f>LEN(D38)</f>
+        <f t="shared" si="0"/>
         <v>92</v>
       </c>
       <c r="D38" t="s">
@@ -1214,7 +1290,7 @@
         <v>5</v>
       </c>
       <c r="C39" s="1">
-        <f>LEN(D39)</f>
+        <f t="shared" si="0"/>
         <v>154</v>
       </c>
       <c r="D39" t="s">
@@ -1229,7 +1305,7 @@
         <v>3</v>
       </c>
       <c r="C40" s="1">
-        <f>LEN(D40)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="D40" t="s">
@@ -1244,7 +1320,7 @@
         <v>5</v>
       </c>
       <c r="C41" s="1">
-        <f>LEN(D41)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="D41" t="s">
@@ -1259,7 +1335,7 @@
         <v>5</v>
       </c>
       <c r="C42" s="1">
-        <f>LEN(D42)</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="D42" t="s">
@@ -1274,7 +1350,7 @@
         <v>3</v>
       </c>
       <c r="C43" s="1">
-        <f>LEN(D43)</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="D43" t="s">
@@ -1283,13 +1359,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C44" s="1">
-        <f>LEN(D44)</f>
+        <f t="shared" si="0"/>
         <v>116</v>
       </c>
       <c r="D44" t="s">
@@ -1298,13 +1374,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C45" s="1">
-        <f>LEN(D45)</f>
+        <f t="shared" si="0"/>
         <v>94</v>
       </c>
       <c r="D45" t="s">
@@ -1313,13 +1389,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C46" s="1">
-        <f>LEN(D46)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="D46" t="s">
@@ -1328,13 +1404,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C47" s="1">
-        <f>LEN(D47)</f>
+        <f t="shared" si="0"/>
         <v>138</v>
       </c>
       <c r="D47" t="s">
@@ -1343,13 +1419,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C48" s="1">
-        <f>LEN(D48)</f>
+        <f t="shared" si="0"/>
         <v>121</v>
       </c>
       <c r="D48" t="s">
@@ -1358,13 +1434,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C49" s="1">
-        <f>LEN(D49)</f>
+        <f t="shared" si="0"/>
         <v>65</v>
       </c>
       <c r="D49" t="s">
@@ -1373,13 +1449,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C50" s="1">
-        <f>LEN(D50)</f>
+        <f t="shared" si="0"/>
         <v>110</v>
       </c>
       <c r="D50" t="s">
@@ -1388,13 +1464,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C51" s="1">
-        <f>LEN(D51)</f>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="D51" t="s">
@@ -1403,1006 +1479,1129 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C52" s="1">
-        <f>LEN(D52)</f>
-        <v>37</v>
+        <f t="shared" si="0"/>
+        <v>46</v>
       </c>
       <c r="D52" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="1">
+        <f t="shared" si="0"/>
+        <v>114</v>
+      </c>
+      <c r="D53" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="1">
-        <f>LEN(D53)</f>
-        <v>114</v>
-      </c>
-      <c r="D53" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+      <c r="C54" s="6">
+        <f t="shared" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="6">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C56" s="6">
+        <f t="shared" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" s="6">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C58" s="6">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="6">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="D59" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C54" s="1">
-        <f>LEN(D54)</f>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C60" s="6">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="9">
+        <v>125</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" s="9">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="11">
+        <v>125</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="11">
+        <v>125</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" s="11">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="11">
+        <v>125</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="11">
+        <f t="shared" si="0"/>
+        <v>118</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="11">
+        <v>125</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65" s="11">
+        <f t="shared" si="0"/>
+        <v>141</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="11">
+        <v>125</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" s="11">
+        <f t="shared" ref="C66:C129" si="1">LEN(D66)</f>
+        <v>120</v>
+      </c>
+      <c r="D66" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D54" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C55" s="1">
-        <f>LEN(D55)</f>
-        <v>44</v>
-      </c>
-      <c r="D55" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C56" s="1">
-        <f>LEN(D56)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C57" s="1">
-        <f>LEN(D57)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C58" s="1">
-        <f>LEN(D58)</f>
-        <v>47</v>
-      </c>
-      <c r="D58" t="s">
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="11">
+        <v>125</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67" s="11">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="11">
+        <v>125</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C68" s="11">
+        <f t="shared" si="1"/>
+        <v>159</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="11">
+        <v>125</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C69" s="11">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="11">
+        <v>125</v>
+      </c>
+      <c r="B70" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="11">
+        <f t="shared" si="1"/>
         <v>62</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="1">
-        <f>LEN(D59)</f>
-        <v>16</v>
-      </c>
-      <c r="D59" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C60" s="1">
-        <f>LEN(D60)</f>
-        <v>15</v>
-      </c>
-      <c r="D60" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C61" s="1">
-        <f>LEN(D61)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C62" s="1">
-        <f>LEN(D62)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C63" s="1">
-        <f>LEN(D63)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C64" s="1">
-        <f>LEN(D64)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C65" s="1">
-        <f>LEN(D65)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C66" s="1">
-        <f>LEN(D66)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C67" s="1">
-        <f>LEN(D67)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C68" s="1">
-        <f>LEN(D68)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C69" s="1">
-        <f>LEN(D69)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C70" s="1">
-        <f>LEN(D70)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C71" s="1">
-        <f>LEN(D71)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C72" s="1">
-        <f>LEN(D72)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C73" s="1">
-        <f>LEN(D73)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D70" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="11">
+        <v>125</v>
+      </c>
+      <c r="B71" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" s="11">
+        <f t="shared" si="1"/>
+        <v>141</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="11">
+        <v>125</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="11">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="D72" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="11">
+        <v>125</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" s="11">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C74" s="1">
-        <f>LEN(D74)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C75" s="1">
-        <f>LEN(D75)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C76" s="1">
-        <f>LEN(D76)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C77" s="1">
-        <f>LEN(D77)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C78" s="1">
-        <f>LEN(D78)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C79" s="1">
-        <f>LEN(D79)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C80" s="1">
-        <f>LEN(D80)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C81" s="1">
-        <f>LEN(D81)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C82" s="1">
-        <f>LEN(D82)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C83" s="1">
-        <f>LEN(D83)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C84" s="1">
-        <f>LEN(D84)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C85" s="1">
-        <f>LEN(D85)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C86" s="1">
-        <f>LEN(D86)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C87" s="1">
-        <f>LEN(D87)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C88" s="1">
-        <f>LEN(D88)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C89" s="1">
-        <f>LEN(D89)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C90" s="1">
-        <f>LEN(D90)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C91" s="1">
-        <f>LEN(D91)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C92" s="1">
-        <f>LEN(D92)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C93" s="1">
-        <f>LEN(D93)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C94" s="1">
-        <f>LEN(D94)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C95" s="1">
-        <f>LEN(D95)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C96" s="1">
-        <f>LEN(D96)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C97" s="1">
-        <f>LEN(D97)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C98" s="1">
-        <f>LEN(D98)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C99" s="1">
-        <f>LEN(D99)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C100" s="1">
-        <f>LEN(D100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C101" s="1">
-        <f>LEN(D101)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C102" s="1">
-        <f>LEN(D102)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C103" s="1">
-        <f>LEN(D103)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C104" s="1">
-        <f>LEN(D104)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="105" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C105" s="1">
-        <f>LEN(D105)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C106" s="1">
-        <f>LEN(D106)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="107" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C107" s="1">
-        <f>LEN(D107)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="108" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C108" s="1">
-        <f>LEN(D108)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="109" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C109" s="1">
-        <f>LEN(D109)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="110" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C110" s="1">
-        <f>LEN(D110)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="111" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C111" s="1">
-        <f>LEN(D111)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="112" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C112" s="1">
-        <f>LEN(D112)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="113" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C113" s="1">
-        <f>LEN(D113)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="114" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C114" s="1">
-        <f>LEN(D114)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="115" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C115" s="1">
-        <f>LEN(D115)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="116" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C116" s="1">
-        <f>LEN(D116)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="117" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C117" s="1">
-        <f>LEN(D117)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="118" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C118" s="1">
-        <f>LEN(D118)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="119" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C119" s="1">
-        <f>LEN(D119)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="120" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C120" s="1">
-        <f>LEN(D120)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="121" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C121" s="1">
-        <f>LEN(D121)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="122" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C122" s="1">
-        <f>LEN(D122)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="123" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C123" s="1">
-        <f>LEN(D123)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="124" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C124" s="1">
-        <f>LEN(D124)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C125" s="1">
-        <f>LEN(D125)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="126" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C126" s="1">
-        <f>LEN(D126)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="127" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C127" s="1">
-        <f>LEN(D127)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="128" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C128" s="1">
-        <f>LEN(D128)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="129" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C129" s="1">
-        <f>LEN(D129)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="130" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C130" s="1">
-        <f>LEN(D130)</f>
+        <f t="shared" ref="C130:C193" si="2">LEN(D130)</f>
         <v>0</v>
       </c>
     </row>
     <row r="131" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C131" s="1">
-        <f>LEN(D131)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="132" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C132" s="1">
-        <f>LEN(D132)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="133" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C133" s="1">
-        <f>LEN(D133)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="134" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C134" s="1">
-        <f>LEN(D134)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="135" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C135" s="1">
-        <f>LEN(D135)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="136" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C136" s="1">
-        <f>LEN(D136)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="137" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C137" s="1">
-        <f>LEN(D137)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="138" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C138" s="1">
-        <f>LEN(D138)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="139" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C139" s="1">
-        <f>LEN(D139)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="140" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C140" s="1">
-        <f>LEN(D140)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="141" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C141" s="1">
-        <f>LEN(D141)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="142" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C142" s="1">
-        <f>LEN(D142)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="143" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C143" s="1">
-        <f>LEN(D143)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="144" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C144" s="1">
-        <f>LEN(D144)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="145" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C145" s="1">
-        <f>LEN(D145)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="146" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C146" s="1">
-        <f>LEN(D146)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="147" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C147" s="1">
-        <f>LEN(D147)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="148" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C148" s="1">
-        <f>LEN(D148)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="149" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C149" s="1">
-        <f>LEN(D149)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="150" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C150" s="1">
-        <f>LEN(D150)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="151" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C151" s="1">
-        <f>LEN(D151)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="152" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C152" s="1">
-        <f>LEN(D152)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="153" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C153" s="1">
-        <f>LEN(D153)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="154" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C154" s="1">
-        <f>LEN(D154)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="155" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C155" s="1">
-        <f>LEN(D155)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="156" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C156" s="1">
-        <f>LEN(D156)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="157" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C157" s="1">
-        <f>LEN(D157)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="158" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C158" s="1">
-        <f>LEN(D158)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="159" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C159" s="1">
-        <f>LEN(D159)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="160" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C160" s="1">
-        <f>LEN(D160)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="161" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C161" s="1">
-        <f>LEN(D161)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="162" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C162" s="1">
-        <f>LEN(D162)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="163" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C163" s="1">
-        <f>LEN(D163)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="164" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C164" s="1">
-        <f>LEN(D164)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="165" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C165" s="1">
-        <f>LEN(D165)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="166" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C166" s="1">
-        <f>LEN(D166)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="167" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C167" s="1">
-        <f>LEN(D167)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="168" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C168" s="1">
-        <f>LEN(D168)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="169" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C169" s="1">
-        <f>LEN(D169)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="170" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C170" s="1">
-        <f>LEN(D170)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="171" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C171" s="1">
-        <f>LEN(D171)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="172" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C172" s="1">
-        <f>LEN(D172)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="173" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C173" s="1">
-        <f>LEN(D173)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="174" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C174" s="1">
-        <f>LEN(D174)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="175" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C175" s="1">
-        <f>LEN(D175)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="176" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C176" s="1">
-        <f>LEN(D176)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="177" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C177" s="1">
-        <f>LEN(D177)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="178" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C178" s="1">
-        <f>LEN(D178)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="179" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C179" s="1">
-        <f>LEN(D179)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="180" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C180" s="1">
-        <f>LEN(D180)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="181" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C181" s="1">
-        <f>LEN(D181)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="182" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C182" s="1">
-        <f>LEN(D182)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="183" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C183" s="1">
-        <f>LEN(D183)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="184" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C184" s="1">
-        <f>LEN(D184)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="185" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C185" s="1">
-        <f>LEN(D185)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="186" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C186" s="1">
-        <f>LEN(D186)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="187" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C187" s="1">
-        <f>LEN(D187)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="188" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C188" s="1">
-        <f>LEN(D188)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="189" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C189" s="1">
-        <f>LEN(D189)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="190" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C190" s="1">
-        <f>LEN(D190)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="191" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C191" s="1">
-        <f>LEN(D191)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="192" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C192" s="1">
-        <f>LEN(D192)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="193" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C193" s="1">
-        <f>LEN(D193)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="194" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C194" s="1">
-        <f>LEN(D194)</f>
+        <f t="shared" ref="C194:C257" si="3">LEN(D194)</f>
         <v>0</v>
       </c>
     </row>
     <row r="195" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C195" s="1">
-        <f>LEN(D195)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="196" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C196" s="1">
-        <f>LEN(D196)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="197" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C197" s="1">
-        <f>LEN(D197)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="198" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C198" s="1">
-        <f>LEN(D198)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="199" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C199" s="1">
-        <f>LEN(D199)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="200" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C200" s="1">
-        <f>LEN(D200)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="201" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C201" s="1">
-        <f>LEN(D201)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="202" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C202" s="1">
-        <f>LEN(D202)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="203" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C203" s="1">
-        <f>LEN(D203)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="204" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C204" s="1">
-        <f>LEN(D204)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="205" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C205" s="1">
-        <f>LEN(D205)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="206" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C206" s="1">
-        <f>LEN(D206)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ChatEngine: update dialogue - make him 900 years old.
</commit_message>
<xml_diff>
--- a/JSON/InGameChatDialogues.xlsx
+++ b/JSON/InGameChatDialogues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F41665F-C4C8-BF46-8160-AAE3D5E21231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1A6F83-5AB7-8D4B-B087-92438B2338F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{BEC1C2E6-1980-8E46-829C-045BE56B3A8A}"/>
+    <workbookView xWindow="0" yWindow="11080" windowWidth="36000" windowHeight="10700" xr2:uid="{BEC1C2E6-1980-8E46-829C-045BE56B3A8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="82">
   <si>
     <t>Profile</t>
   </si>
@@ -53,33 +53,12 @@
     <t>Hero</t>
   </si>
   <si>
-    <t>…and that's the whole story! So what's our game plan?</t>
-  </si>
-  <si>
     <t>Trainer</t>
   </si>
   <si>
-    <t>I suspect she is being held captive in the dragon's lair, so it's important we move fast. I am going to guide you there, so pay attention.</t>
-  </si>
-  <si>
-    <t>How do you know that's where they've taken her??</t>
-  </si>
-  <si>
-    <t>Don't worry about it... OK. The lair is buried miles beneath the Earth's surface, and the only way to reach it is to solve logic puzzles.</t>
-  </si>
-  <si>
-    <t>Makes no sense, but go on...</t>
-  </si>
-  <si>
-    <t>There are 500 levels in total you will have to solve, each with increasing difficulty.</t>
-  </si>
-  <si>
     <t>500 levels?!! What do I get if I win?</t>
   </si>
   <si>
-    <t>You save the world!!! Now where was I... Oh yeah, the goal for each level is to get to the gate in under a certain number of moves.</t>
-  </si>
-  <si>
     <t>You can move to any available panel on your left, right, above, and below. Simply tap the panel to move there. Diagonal moves are not allowed.</t>
   </si>
   <si>
@@ -104,9 +83,6 @@
     <t>Since there are no hammers in this level, you'll just have to go around them.</t>
   </si>
   <si>
-    <t>Well then, that was pointless.</t>
-  </si>
-  <si>
     <t>Oh, and one more thing... hammers can only be used once before breaking, so plan your moves ahead of time.</t>
   </si>
   <si>
@@ -125,9 +101,6 @@
     <t>Are those things safe?</t>
   </si>
   <si>
-    <t>We're about to find out. Good luck!</t>
-  </si>
-  <si>
     <t>.......</t>
   </si>
   <si>
@@ -149,9 +122,6 @@
     <t>Lemme guess, I can only use the sword once before it breaks?</t>
   </si>
   <si>
-    <t>B-I-N-G-O!!! Oh whoops, I was playing Bingo with my grams. Yep, one sword per dragon.</t>
-  </si>
-  <si>
     <t>Ice, ice, baby! Step on this and you'll slide until you hit either an obstacle or the edge of the level.</t>
   </si>
   <si>
@@ -242,9 +212,6 @@
     <t>Ok, ok. I'll be ready. I already know how to use swords and hammers. Nothing can stop me!</t>
   </si>
   <si>
-    <t>Well yeah, after I saw a friggin' dragon swoop down from a blood soaked sky and snatch a 7 year old girl, you appeared almost out of nowhere.</t>
-  </si>
-  <si>
     <t>Look, if it's the old man comment, everybody gets old. It's just an inevitability of life. I'm 16 so everyone looks old to me.</t>
   </si>
   <si>
@@ -260,18 +227,9 @@
     <t>You'll never find her... You can keep trying, but she serves another purpose now...</t>
   </si>
   <si>
-    <t>Such a shame. So lost. One day you'll know the truth...</t>
-  </si>
-  <si>
     <t>...</t>
   </si>
   <si>
-    <t>ONE THOUSAND??!! What are you, like a wizard or something? Wait... ARE YOU?!?! Because I'm not surprised by anything anymore at this point...</t>
-  </si>
-  <si>
-    <t>No, it's not that. I'm 1,000 years old. I AM old. I'm just thinking about how important it is we complete the mission.</t>
-  </si>
-  <si>
     <t>I mean you don't look a day over 800 to be honest...</t>
   </si>
   <si>
@@ -281,7 +239,52 @@
     <t>There's a lot you must learn to prepare you for the upcoming battle to save your world and the worlds beyond your world.</t>
   </si>
   <si>
-    <t>Wow.. 1,000 years old. I have soooo many questions...</t>
+    <t>PUZL BOY: ...then the dragon swooped down and carried her away! So... what's our game plan? Also I didn't catch your name.</t>
+  </si>
+  <si>
+    <t>MARLIN: I am Marlin. I suspect she is being held captive in the dragon's lair. We must move quickly. I'm going to guide you there, so pay attention.</t>
+  </si>
+  <si>
+    <t>Marlin, like the fish??? How do you know that's where they've taken her?</t>
+  </si>
+  <si>
+    <t>Marlin like the magician. Don't worry about it... OK. The lair is buried miles beneath the Earth's surface, and the only way to reach it is to solve logic puzzles.</t>
+  </si>
+  <si>
+    <t>A marlin is a fish... You're thinking of Merlin the Magician. Is that your name? Merlin?</t>
+  </si>
+  <si>
+    <t>I think I know my own name. Listen!! There are 500 levels in total you will have to solve, each with increasing difficulty.</t>
+  </si>
+  <si>
+    <t>You save the world!!! Geez! Now where was I... Oh yeah, the goal for each level is to get to the gate in under a certain number of moves.</t>
+  </si>
+  <si>
+    <t>Ah well, gotta get my steps in.</t>
+  </si>
+  <si>
+    <t>Ummmmmmm yeah, sure! I've tested it myself hundreds of times.</t>
+  </si>
+  <si>
+    <t>Now you're getting it!</t>
+  </si>
+  <si>
+    <t>No, it's not that. I'm 900 years old. I AM old. I'm just thinking about how important it is we complete the mission.</t>
+  </si>
+  <si>
+    <t>NINE HUNDRED??!! What are you, like a wizard or something? \"Marlin the Fishy Wizard...\"</t>
+  </si>
+  <si>
+    <t>Wait... ARE YOU REALLY A WIZARD?!?! Because I'm not surprised by anything anymore at this point…</t>
+  </si>
+  <si>
+    <t>Well yeah, after I saw a freakin' dragon swoop down from a blood soaked sky and snatch a 7 year old girl, ...then you appeared almost out of nowhere!</t>
+  </si>
+  <si>
+    <t>Wow.. 900 years old. I have soooo many questions...</t>
+  </si>
+  <si>
+    <t>Such a shame. So lost. One day you'll understand...</t>
   </si>
 </sst>
 </file>
@@ -355,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -375,11 +378,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -696,13 +695,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C796D1D-820D-5D44-A707-B56EAA85DA7C}">
-  <dimension ref="A1:D206"/>
+  <dimension ref="A1:D207"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D66" sqref="D66"/>
+      <selection pane="bottomRight" activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -721,7 +720,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -736,10 +735,10 @@
       </c>
       <c r="C2" s="1">
         <f t="shared" ref="C2:C65" si="0">LEN(D2)</f>
-        <v>53</v>
+        <v>122</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -747,14 +746,14 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1">
         <f t="shared" si="0"/>
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -766,10 +765,10 @@
       </c>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -777,14 +776,14 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -796,10 +795,10 @@
       </c>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -807,14 +806,14 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="0"/>
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -829,7 +828,7 @@
         <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -837,14 +836,14 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="0"/>
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -852,14 +851,14 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="0"/>
         <v>142</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -867,14 +866,14 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" si="0"/>
         <v>124</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -882,14 +881,14 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -904,7 +903,7 @@
         <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -912,14 +911,14 @@
         <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -927,14 +926,14 @@
         <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="0"/>
         <v>107</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -949,7 +948,7 @@
         <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -957,14 +956,14 @@
         <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -976,10 +975,10 @@
       </c>
       <c r="C18" s="1">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -987,14 +986,14 @@
         <v>8</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" s="1">
         <f t="shared" si="0"/>
         <v>106</v>
       </c>
       <c r="D19" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1002,14 +1001,14 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" si="0"/>
         <v>114</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1017,14 +1016,14 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1039,7 +1038,7 @@
         <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1047,14 +1046,14 @@
         <v>34</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23" s="1">
         <f t="shared" si="0"/>
         <v>107</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1069,7 +1068,7 @@
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1077,14 +1076,14 @@
         <v>34</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25" s="1">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D25" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1099,7 +1098,7 @@
         <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1114,7 +1113,7 @@
         <v>58</v>
       </c>
       <c r="D27" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1122,14 +1121,14 @@
         <v>51</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" s="1">
         <f t="shared" si="0"/>
         <v>126</v>
       </c>
       <c r="D28" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1144,7 +1143,7 @@
         <v>47</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1152,14 +1151,14 @@
         <v>51</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" s="1">
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
       <c r="D30" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1167,14 +1166,14 @@
         <v>51</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31" s="1">
         <f t="shared" si="0"/>
         <v>116</v>
       </c>
       <c r="D31" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1182,14 +1181,14 @@
         <v>51</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32" s="1">
         <f t="shared" si="0"/>
         <v>112</v>
       </c>
       <c r="D32" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1204,7 +1203,7 @@
         <v>60</v>
       </c>
       <c r="D33" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1212,14 +1211,14 @@
         <v>51</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C34" s="1">
         <f t="shared" si="0"/>
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="D34" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1227,14 +1226,14 @@
         <v>76</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C35" s="1">
         <f t="shared" si="0"/>
         <v>104</v>
       </c>
       <c r="D35" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1242,14 +1241,14 @@
         <v>76</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C36" s="1">
         <f t="shared" si="0"/>
         <v>96</v>
       </c>
       <c r="D36" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1264,7 +1263,7 @@
         <v>30</v>
       </c>
       <c r="D37" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1272,14 +1271,14 @@
         <v>76</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C38" s="1">
         <f t="shared" si="0"/>
         <v>92</v>
       </c>
       <c r="D38" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1287,14 +1286,14 @@
         <v>100</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C39" s="1">
         <f t="shared" si="0"/>
         <v>154</v>
       </c>
       <c r="D39" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1309,7 +1308,7 @@
         <v>35</v>
       </c>
       <c r="D40" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1317,14 +1316,14 @@
         <v>100</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C41" s="1">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="D41" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1332,14 +1331,14 @@
         <v>100</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42" s="1">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="D42" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1354,12 +1353,12 @@
         <v>60</v>
       </c>
       <c r="D43" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>3</v>
@@ -1369,27 +1368,27 @@
         <v>116</v>
       </c>
       <c r="D44" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C45" s="1">
         <f t="shared" si="0"/>
         <v>94</v>
       </c>
       <c r="D45" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>3</v>
@@ -1399,87 +1398,87 @@
         <v>21</v>
       </c>
       <c r="D46" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C47" s="1">
         <f t="shared" si="0"/>
         <v>138</v>
       </c>
       <c r="D47" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C48" s="1">
         <f t="shared" si="0"/>
         <v>121</v>
       </c>
       <c r="D48" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C49" s="1">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
       <c r="D49" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C50" s="1">
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
       <c r="D50" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C51" s="1">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="D51" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>3</v>
@@ -1489,127 +1488,127 @@
         <v>46</v>
       </c>
       <c r="D52" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C53" s="1">
         <f t="shared" si="0"/>
         <v>114</v>
       </c>
       <c r="D53" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C54" s="6">
         <f t="shared" si="0"/>
         <v>83</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C55" s="6">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B56" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" s="6">
+        <f t="shared" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="D56" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="C56" s="6">
-        <f t="shared" si="0"/>
-        <v>83</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C57" s="6">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C58" s="6">
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C59" s="6">
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C60" s="6">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1623,985 +1622,1000 @@
         <f t="shared" si="0"/>
         <v>96</v>
       </c>
-      <c r="D61" s="10" t="s">
+      <c r="D61" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>125</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>125</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" s="1">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>125</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" s="1">
+        <f t="shared" si="0"/>
+        <v>116</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>125</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65" s="1">
+        <f t="shared" si="0"/>
+        <v>89</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>125</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66" s="1">
+        <f t="shared" ref="C66" si="1">LEN(D66)</f>
+        <v>96</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>125</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" s="1">
+        <f t="shared" ref="C67:C130" si="2">LEN(D67)</f>
+        <v>120</v>
+      </c>
+      <c r="D67" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="11">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
         <v>125</v>
       </c>
-      <c r="B62" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C62" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="D62" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="11">
+      <c r="B68" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68" s="1">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
         <v>125</v>
       </c>
-      <c r="B63" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C63" s="11">
-        <f t="shared" si="0"/>
-        <v>126</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="11">
+      <c r="B69" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C69" s="1">
+        <f t="shared" si="2"/>
+        <v>159</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
         <v>125</v>
       </c>
-      <c r="B64" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C64" s="11">
-        <f t="shared" si="0"/>
-        <v>118</v>
-      </c>
-      <c r="D64" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="11">
+      <c r="B70" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" s="1">
+        <f t="shared" si="2"/>
+        <v>89</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
         <v>125</v>
       </c>
-      <c r="B65" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C65" s="11">
-        <f t="shared" si="0"/>
-        <v>141</v>
-      </c>
-      <c r="D65" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="11">
+      <c r="B71" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" s="1">
+        <f t="shared" si="2"/>
+        <v>62</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
         <v>125</v>
       </c>
-      <c r="B66" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C66" s="11">
-        <f t="shared" ref="C66:C129" si="1">LEN(D66)</f>
-        <v>120</v>
-      </c>
-      <c r="D66" s="10" t="s">
+      <c r="B72" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72" s="1">
+        <f t="shared" si="2"/>
+        <v>149</v>
+      </c>
+      <c r="D72" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="11">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
         <v>125</v>
       </c>
-      <c r="B67" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C67" s="11">
-        <f t="shared" si="1"/>
-        <v>52</v>
-      </c>
-      <c r="D67" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="11">
+      <c r="B73" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C73" s="1">
+        <f t="shared" si="2"/>
+        <v>87</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
         <v>125</v>
       </c>
-      <c r="B68" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C68" s="11">
-        <f t="shared" si="1"/>
-        <v>159</v>
-      </c>
-      <c r="D68" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="11">
-        <v>125</v>
-      </c>
-      <c r="B69" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C69" s="11">
-        <f t="shared" si="1"/>
-        <v>89</v>
-      </c>
-      <c r="D69" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="11">
-        <v>125</v>
-      </c>
-      <c r="B70" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="11">
-        <f t="shared" si="1"/>
-        <v>62</v>
-      </c>
-      <c r="D70" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="11">
-        <v>125</v>
-      </c>
-      <c r="B71" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C71" s="11">
-        <f t="shared" si="1"/>
-        <v>141</v>
-      </c>
-      <c r="D71" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="11">
-        <v>125</v>
-      </c>
-      <c r="B72" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C72" s="11">
-        <f t="shared" si="1"/>
-        <v>87</v>
-      </c>
-      <c r="D72" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="11">
-        <v>125</v>
-      </c>
-      <c r="B73" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C73" s="11">
-        <f t="shared" si="1"/>
-        <v>53</v>
-      </c>
-      <c r="D73" s="10" t="s">
+      <c r="B74" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" s="1">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="D74" s="5" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C74" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C75" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C76" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C77" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C78" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C79" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C80" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C81" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C82" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C83" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C84" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C85" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C86" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C87" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C88" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C89" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C90" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C91" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C92" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C93" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C94" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C95" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C96" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C97" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C98" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C99" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C100" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C101" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C102" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C103" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C104" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="105" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C105" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C106" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="107" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C107" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="108" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C108" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="109" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C109" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="110" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C110" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="111" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C111" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="112" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C112" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="113" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C113" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="114" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C114" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="115" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C115" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="116" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C116" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="117" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C117" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="118" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C118" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="119" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C119" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="120" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C120" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="121" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C121" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="122" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C122" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="123" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C123" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="124" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C124" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C125" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="126" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C126" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="127" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C127" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="128" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C128" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="129" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C129" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="130" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C130" s="1">
-        <f t="shared" ref="C130:C193" si="2">LEN(D130)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="131" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C131" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="C131:C194" si="3">LEN(D131)</f>
         <v>0</v>
       </c>
     </row>
     <row r="132" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C132" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="133" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C133" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="134" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C134" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="135" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C135" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="136" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C136" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="137" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C137" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="138" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C138" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="139" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C139" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="140" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C140" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="141" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C141" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="142" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C142" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="143" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C143" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="144" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C144" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="145" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C145" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="146" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C146" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="147" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C147" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="148" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C148" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="149" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C149" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="150" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C150" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="151" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C151" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="152" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C152" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="153" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C153" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="154" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C154" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="155" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C155" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="156" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C156" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="157" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C157" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="158" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C158" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="159" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C159" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="160" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C160" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="161" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C161" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="162" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C162" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="163" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C163" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="164" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C164" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="165" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C165" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="166" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C166" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="167" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C167" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="168" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C168" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="169" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C169" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="170" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C170" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="171" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C171" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="172" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C172" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="173" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C173" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="174" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C174" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="175" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C175" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="176" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C176" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="177" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C177" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="178" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C178" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="179" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C179" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="180" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C180" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="181" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C181" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="182" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C182" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="183" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C183" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="184" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C184" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="185" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C185" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="186" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C186" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="187" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C187" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="188" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C188" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="189" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C189" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="190" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C190" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="191" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C191" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="192" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C192" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="193" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C193" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="194" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C194" s="1">
-        <f t="shared" ref="C194:C257" si="3">LEN(D194)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="195" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C195" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="C195:C207" si="4">LEN(D195)</f>
         <v>0</v>
       </c>
     </row>
     <row r="196" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C196" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="197" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C197" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="198" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C198" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="199" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C199" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="200" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C200" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="201" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C201" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="202" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C202" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="203" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C203" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="204" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C204" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="205" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C205" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="206" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C206" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C207" s="1">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor. Change name from Eldoria to Vaeloria. Update "what's wrong" dialogue from LV 125 to 131.
</commit_message>
<xml_diff>
--- a/JSON/InGameChatDialogues.xlsx
+++ b/JSON/InGameChatDialogues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1A6F83-5AB7-8D4B-B087-92438B2338F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CE8A12-D857-3D42-B8FB-4E6564B49DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="11080" windowWidth="36000" windowHeight="10700" xr2:uid="{BEC1C2E6-1980-8E46-829C-045BE56B3A8A}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{BEC1C2E6-1980-8E46-829C-045BE56B3A8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -698,10 +698,10 @@
   <dimension ref="A1:D207"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D61" sqref="D61"/>
+      <selection pane="bottomRight" activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1613,7 +1613,7 @@
     </row>
     <row r="61" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="9">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>3</v>
@@ -1627,8 +1627,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="1">
-        <v>125</v>
+      <c r="A62" s="9">
+        <v>131</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>4</v>
@@ -1642,8 +1642,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="1">
-        <v>125</v>
+      <c r="A63" s="9">
+        <v>131</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>3</v>
@@ -1657,8 +1657,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="1">
-        <v>125</v>
+      <c r="A64" s="9">
+        <v>131</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>4</v>
@@ -1672,8 +1672,8 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="1">
-        <v>125</v>
+      <c r="A65" s="9">
+        <v>131</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>3</v>
@@ -1687,8 +1687,8 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="1">
-        <v>125</v>
+      <c r="A66" s="9">
+        <v>131</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>3</v>
@@ -1702,8 +1702,8 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="1">
-        <v>125</v>
+      <c r="A67" s="9">
+        <v>131</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>4</v>
@@ -1717,8 +1717,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="1">
-        <v>125</v>
+      <c r="A68" s="9">
+        <v>131</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>3</v>
@@ -1732,8 +1732,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="1">
-        <v>125</v>
+      <c r="A69" s="9">
+        <v>131</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>4</v>
@@ -1747,8 +1747,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="1">
-        <v>125</v>
+      <c r="A70" s="9">
+        <v>131</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>3</v>
@@ -1762,8 +1762,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="1">
-        <v>125</v>
+      <c r="A71" s="9">
+        <v>131</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>4</v>
@@ -1777,8 +1777,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="1">
-        <v>125</v>
+      <c r="A72" s="9">
+        <v>131</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>3</v>
@@ -1792,8 +1792,8 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="1">
-        <v>125</v>
+      <c r="A73" s="9">
+        <v>131</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>4</v>
@@ -1807,8 +1807,8 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="1">
-        <v>125</v>
+      <c r="A74" s="9">
+        <v>131</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>3</v>

</xml_diff>